<commit_message>
updated obj function, added constraint
</commit_message>
<xml_diff>
--- a/NuclearData.xlsx
+++ b/NuclearData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\Uni\OR-INF\operations_oppenheimer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F79B706-6A42-4161-AA9D-86295BD57ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD16212E-EB94-41DA-8C22-CFCFE02C1CE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CISF" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="24">
   <si>
     <t>Hot Cell 1</t>
   </si>
@@ -107,6 +107,12 @@
   </si>
   <si>
     <t>Hot_cell_operating_costs</t>
+  </si>
+  <si>
+    <t>prebuild</t>
+  </si>
+  <si>
+    <t>Superstorage</t>
   </si>
 </sst>
 </file>
@@ -484,15 +490,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -502,38 +508,64 @@
       <c r="C1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
-        <v>5000</v>
+        <v>420</v>
       </c>
       <c r="C2">
         <v>999</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>5000</v>
+        <v>420</v>
       </c>
       <c r="C3">
         <v>999</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>5000</v>
+        <v>420</v>
       </c>
       <c r="C4">
         <v>999</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5">
+        <v>500</v>
+      </c>
+      <c r="C5">
+        <v>999</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -546,7 +578,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -688,54 +720,44 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2">
         <v>5000</v>
       </c>
-      <c r="C2">
-        <v>5000</v>
-      </c>
-      <c r="D2">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3">
         <v>8000</v>
       </c>
-      <c r="C3">
-        <v>8000</v>
-      </c>
-      <c r="D3">
-        <v>300</v>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>2000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>